<commit_message>
Handle same names + Convert to SubjectID
</commit_message>
<xml_diff>
--- a/Main_DB.xlsx
+++ b/Main_DB.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Subject_Name</t>
   </si>
@@ -38,9 +38,6 @@
   </si>
   <si>
     <t>gopal_2_3_4</t>
-  </si>
-  <si>
-    <t>gopal_2_3_4_5</t>
   </si>
 </sst>
 </file>
@@ -398,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -460,14 +457,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>